<commit_message>
The data on the passport and the employee's patent was recorded in the notice of conclusion and termination
</commit_message>
<xml_diff>
--- a/document_generation/document_generation_app/document_templates/notice_conclusion.xlsx
+++ b/document_generation/document_generation_app/document_templates/notice_conclusion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Document_generation_service\document_generation\document_generation_app\document_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C644EA-1B97-4FCA-9CB6-6583C57D8D07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4F5569-BF8F-413A-95FE-C1D9CE80B4E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="122">
   <si>
     <t>Приложение № 7</t>
   </si>
@@ -49,22 +49,13 @@
     <t>Т</t>
   </si>
   <si>
-    <t>Д</t>
-  </si>
-  <si>
     <t>Е</t>
-  </si>
-  <si>
-    <t>Л</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>П</t>
-  </si>
-  <si>
-    <t>В</t>
   </si>
   <si>
     <t>Р</t>
@@ -76,28 +67,13 @@
     <t>А</t>
   </si>
   <si>
-    <t>М</t>
-  </si>
-  <si>
     <t>И</t>
-  </si>
-  <si>
-    <t>Г</t>
-  </si>
-  <si>
-    <t>У</t>
-  </si>
-  <si>
-    <t>К</t>
   </si>
   <si>
     <t>Н</t>
   </si>
   <si>
     <t>Й</t>
-  </si>
-  <si>
-    <t>Б</t>
   </si>
   <si>
     <t>(наименование территориального органа МВД России на региональном уровне)</t>
@@ -207,21 +183,6 @@
     <t>юридического лица, для индивидуальных предпринимателей — государственный регистрационный</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>номер записи в Едином государственном реестре индивидуальных предпринимателей,</t>
   </si>
   <si>
@@ -237,16 +198,7 @@
     <t>наименование документа, удостоверяющего личность, его серия и номер, кем и когда выдан)</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>(номер свидетельства о постановке на учет в налоговом органе, ИНН (при наличии), КПП (при наличии)</t>
-  </si>
-  <si>
-    <t>Ж</t>
   </si>
   <si>
     <t>(место нахождения (для физического лица — адрес фактического места жительства) работодателя</t>
@@ -267,16 +219,10 @@
     <t>2.1. Фамилия</t>
   </si>
   <si>
-    <t>З</t>
-  </si>
-  <si>
     <t>2.2. Имя</t>
   </si>
   <si>
     <t>2.3. Отчество</t>
-  </si>
-  <si>
-    <t>Ч</t>
   </si>
   <si>
     <t>(при наличии)</t>
@@ -353,9 +299,6 @@
   </si>
   <si>
     <t>с</t>
-  </si>
-  <si>
-    <t>по</t>
   </si>
   <si>
     <t>3.1. Трудовая деятельность осуществляется иностранным гражданином (лицом без гражданства) без разрешения на работу или патента на основании (не заполняется в случае осуществления трудовой деятельности на основании разрешения на работу или патента)</t>
@@ -1121,8 +1064,8 @@
   </sheetPr>
   <dimension ref="A1:BS208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="X203" sqref="X203:AJ203"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="AQ115" sqref="AQ115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1610,7 +1553,7 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
@@ -1618,7 +1561,7 @@
       <c r="O11" s="20"/>
       <c r="P11" s="20"/>
       <c r="Q11" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R11" s="20"/>
       <c r="S11" s="20"/>
@@ -1638,7 +1581,7 @@
       <c r="AG11" s="20"/>
       <c r="AH11" s="20"/>
       <c r="AI11" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AJ11" s="20"/>
       <c r="AK11" s="20"/>
@@ -1658,7 +1601,7 @@
       <c r="AY11" s="20"/>
       <c r="AZ11" s="20"/>
       <c r="BA11" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BB11" s="20"/>
       <c r="BC11" s="20"/>
@@ -1670,7 +1613,7 @@
       <c r="BI11" s="20"/>
       <c r="BJ11" s="20"/>
       <c r="BK11" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BL11" s="20"/>
       <c r="BM11" s="20"/>
@@ -1761,7 +1704,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -1769,7 +1712,7 @@
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
       <c r="M13" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N13" s="20"/>
       <c r="O13" s="20"/>
@@ -1797,7 +1740,7 @@
       <c r="AK13" s="20"/>
       <c r="AL13" s="20"/>
       <c r="AM13" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AN13" s="20"/>
       <c r="AO13" s="20"/>
@@ -1813,7 +1756,7 @@
       <c r="AY13" s="20"/>
       <c r="AZ13" s="20"/>
       <c r="BA13" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BB13" s="20"/>
       <c r="BC13" s="20"/>
@@ -1980,7 +1923,7 @@
     </row>
     <row r="16" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -2127,24 +2070,24 @@
     </row>
     <row r="18" spans="1:71" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="BF18" s="11" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="BH18" s="20" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="BI18" s="20"/>
       <c r="BK18" s="10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="BO18" s="20" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="BP18" s="20"/>
       <c r="BQ18" s="10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:71" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
@@ -2222,31 +2165,31 @@
     </row>
     <row r="20" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B20" s="20"/>
       <c r="D20" s="7" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="AI20" s="20"/>
       <c r="AJ20" s="20"/>
       <c r="AL20" s="7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AL21" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AL22" s="7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AL23" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:71" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
@@ -2326,17 +2269,17 @@
       <c r="A25" s="20"/>
       <c r="B25" s="20"/>
       <c r="D25" s="7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="AI25" s="20"/>
       <c r="AJ25" s="20"/>
       <c r="AL25" s="7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AL26" s="7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:71" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
@@ -2416,17 +2359,17 @@
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="D28" s="7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="AI28" s="20"/>
       <c r="AJ28" s="20"/>
       <c r="AL28" s="7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:71" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
@@ -2506,17 +2449,17 @@
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
       <c r="D31" s="7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI31" s="20"/>
       <c r="AJ31" s="20"/>
       <c r="AL31" s="7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D32" s="7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:71" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
@@ -2594,7 +2537,7 @@
     </row>
     <row r="34" spans="1:71" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
@@ -2730,23 +2673,23 @@
       <c r="AQ36" s="22"/>
       <c r="AT36" s="7"/>
       <c r="AU36" s="20" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AV36" s="20"/>
       <c r="AW36" s="20" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AX36" s="20"/>
       <c r="AY36" s="20" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="AZ36" s="20"/>
       <c r="BA36" s="20" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="BB36" s="20"/>
       <c r="BC36" s="20" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="BD36" s="20"/>
       <c r="BE36" s="20"/>
@@ -2766,7 +2709,7 @@
     </row>
     <row r="37" spans="1:71" s="12" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AU37" s="23" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="AV37" s="23"/>
       <c r="AW37" s="23"/>
@@ -2867,7 +2810,7 @@
     </row>
     <row r="39" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:71" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
@@ -2951,7 +2894,7 @@
       <c r="E41" s="20"/>
       <c r="F41" s="20"/>
       <c r="G41" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
@@ -3309,7 +3252,7 @@
     </row>
     <row r="46" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="23" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B46" s="23"/>
       <c r="C46" s="23"/>
@@ -3383,7 +3326,7 @@
     </row>
     <row r="47" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="24" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
@@ -3457,7 +3400,7 @@
     </row>
     <row r="48" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="24" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B48" s="24"/>
       <c r="C48" s="24"/>
@@ -3676,7 +3619,7 @@
     </row>
     <row r="51" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="23" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B51" s="23"/>
       <c r="C51" s="23"/>
@@ -3750,7 +3693,7 @@
     </row>
     <row r="52" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B52" s="24"/>
       <c r="C52" s="24"/>
@@ -3969,7 +3912,7 @@
     </row>
     <row r="55" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="23" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
@@ -4043,7 +3986,7 @@
     </row>
     <row r="56" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="24" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B56" s="24"/>
       <c r="C56" s="24"/>
@@ -4262,7 +4205,7 @@
     </row>
     <row r="59" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="23" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="23"/>
@@ -4554,7 +4497,7 @@
     </row>
     <row r="63" spans="1:71" s="2" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="25" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B63" s="25"/>
       <c r="C63" s="25"/>
@@ -4702,7 +4645,7 @@
     </row>
     <row r="65" spans="1:71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="26" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B65" s="26"/>
       <c r="C65" s="26"/>
@@ -4922,7 +4865,7 @@
     </row>
     <row r="68" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="23" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B68" s="23"/>
       <c r="C68" s="23"/>
@@ -5141,7 +5084,7 @@
     </row>
     <row r="71" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="23" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B71" s="23"/>
       <c r="C71" s="23"/>
@@ -5360,7 +5303,7 @@
     </row>
     <row r="74" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="23" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B74" s="23"/>
       <c r="C74" s="23"/>
@@ -5537,7 +5480,7 @@
       <c r="AC76" s="20"/>
       <c r="AD76" s="20"/>
       <c r="AE76" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AF76" s="20"/>
       <c r="AG76" s="20"/>
@@ -5581,7 +5524,7 @@
     </row>
     <row r="77" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="23" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B77" s="23"/>
       <c r="C77" s="23"/>
@@ -5746,7 +5689,7 @@
       <c r="Q79" s="20"/>
       <c r="R79" s="20"/>
       <c r="S79" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="T79" s="20"/>
       <c r="U79" s="20"/>
@@ -5802,7 +5745,7 @@
     </row>
     <row r="80" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="23" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B80" s="23"/>
       <c r="C80" s="23"/>
@@ -6021,7 +5964,7 @@
     </row>
     <row r="83" spans="1:71" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="23" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B83" s="23"/>
       <c r="C83" s="23"/>
@@ -6168,7 +6111,7 @@
     </row>
     <row r="85" spans="1:71" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="U85" s="20"/>
       <c r="V85" s="20"/>
@@ -6296,7 +6239,7 @@
     </row>
     <row r="87" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="22" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B87" s="22"/>
       <c r="C87" s="22"/>
@@ -6590,35 +6533,21 @@
     </row>
     <row r="91" spans="1:71" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="O91" s="20" t="s">
-        <v>22</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="O91" s="20"/>
       <c r="P91" s="20"/>
-      <c r="Q91" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q91" s="20"/>
       <c r="R91" s="20"/>
-      <c r="S91" s="20" t="s">
-        <v>14</v>
-      </c>
+      <c r="S91" s="20"/>
       <c r="T91" s="20"/>
-      <c r="U91" s="20" t="s">
-        <v>80</v>
-      </c>
+      <c r="U91" s="20"/>
       <c r="V91" s="20"/>
-      <c r="W91" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="W91" s="20"/>
       <c r="X91" s="20"/>
-      <c r="Y91" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y91" s="20"/>
       <c r="Z91" s="20"/>
-      <c r="AA91" s="20" t="s">
-        <v>13</v>
-      </c>
+      <c r="AA91" s="20"/>
       <c r="AB91" s="20"/>
       <c r="AC91" s="20"/>
       <c r="AD91" s="20"/>
@@ -6738,27 +6667,17 @@
     </row>
     <row r="93" spans="1:71" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="O93" s="20" t="s">
-        <v>14</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="O93" s="20"/>
       <c r="P93" s="20"/>
-      <c r="Q93" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q93" s="20"/>
       <c r="R93" s="20"/>
-      <c r="S93" s="20" t="s">
-        <v>15</v>
-      </c>
+      <c r="S93" s="20"/>
       <c r="T93" s="20"/>
-      <c r="U93" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="U93" s="20"/>
       <c r="V93" s="20"/>
-      <c r="W93" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="W93" s="20"/>
       <c r="X93" s="20"/>
       <c r="Y93" s="20"/>
       <c r="Z93" s="20"/>
@@ -6882,43 +6801,25 @@
     </row>
     <row r="95" spans="1:71" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="O95" s="20" t="s">
-        <v>22</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="O95" s="20"/>
       <c r="P95" s="20"/>
-      <c r="Q95" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="Q95" s="20"/>
       <c r="R95" s="20"/>
-      <c r="S95" s="20" t="s">
-        <v>80</v>
-      </c>
+      <c r="S95" s="20"/>
       <c r="T95" s="20"/>
-      <c r="U95" s="20" t="s">
-        <v>14</v>
-      </c>
+      <c r="U95" s="20"/>
       <c r="V95" s="20"/>
-      <c r="W95" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="W95" s="20"/>
       <c r="X95" s="20"/>
-      <c r="Y95" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="Y95" s="20"/>
       <c r="Z95" s="20"/>
-      <c r="AA95" s="20" t="s">
-        <v>13</v>
-      </c>
+      <c r="AA95" s="20"/>
       <c r="AB95" s="20"/>
-      <c r="AC95" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="AC95" s="20"/>
       <c r="AD95" s="20"/>
-      <c r="AE95" s="20" t="s">
-        <v>83</v>
-      </c>
+      <c r="AE95" s="20"/>
       <c r="AF95" s="20"/>
       <c r="AG95" s="20"/>
       <c r="AH95" s="20"/>
@@ -6961,7 +6862,7 @@
     </row>
     <row r="96" spans="1:71" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="1:71" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7039,52 +6940,30 @@
     </row>
     <row r="98" spans="1:71" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="P98" s="15"/>
-      <c r="Q98" s="20" t="s">
-        <v>7</v>
-      </c>
+      <c r="Q98" s="20"/>
       <c r="R98" s="20"/>
-      <c r="S98" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="S98" s="20"/>
       <c r="T98" s="20"/>
-      <c r="U98" s="20" t="s">
-        <v>8</v>
-      </c>
+      <c r="U98" s="20"/>
       <c r="V98" s="20"/>
-      <c r="W98" s="20" t="s">
-        <v>73</v>
-      </c>
+      <c r="W98" s="20"/>
       <c r="X98" s="20"/>
-      <c r="Y98" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="Y98" s="20"/>
       <c r="Z98" s="20"/>
-      <c r="AA98" s="20" t="s">
-        <v>21</v>
-      </c>
+      <c r="AA98" s="20"/>
       <c r="AB98" s="20"/>
-      <c r="AC98" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="AC98" s="20"/>
       <c r="AD98" s="20"/>
-      <c r="AE98" s="20" t="s">
-        <v>15</v>
-      </c>
+      <c r="AE98" s="20"/>
       <c r="AF98" s="20"/>
-      <c r="AG98" s="20" t="s">
-        <v>7</v>
-      </c>
+      <c r="AG98" s="20"/>
       <c r="AH98" s="20"/>
-      <c r="AI98" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="AI98" s="20"/>
       <c r="AJ98" s="20"/>
-      <c r="AK98" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="AK98" s="20"/>
       <c r="AL98" s="20"/>
       <c r="AM98" s="20"/>
       <c r="AN98" s="20"/>
@@ -7194,52 +7073,30 @@
     </row>
     <row r="100" spans="1:71" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="V100" s="15"/>
-      <c r="W100" s="20" t="s">
-        <v>7</v>
-      </c>
+      <c r="W100" s="20"/>
       <c r="X100" s="20"/>
-      <c r="Y100" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="Y100" s="20"/>
       <c r="Z100" s="20"/>
-      <c r="AA100" s="20" t="s">
-        <v>8</v>
-      </c>
+      <c r="AA100" s="20"/>
       <c r="AB100" s="20"/>
-      <c r="AC100" s="20" t="s">
-        <v>73</v>
-      </c>
+      <c r="AC100" s="20"/>
       <c r="AD100" s="20"/>
-      <c r="AE100" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="AE100" s="20"/>
       <c r="AF100" s="20"/>
-      <c r="AG100" s="20" t="s">
-        <v>21</v>
-      </c>
+      <c r="AG100" s="20"/>
       <c r="AH100" s="20"/>
-      <c r="AI100" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="AI100" s="20"/>
       <c r="AJ100" s="20"/>
-      <c r="AK100" s="20" t="s">
-        <v>15</v>
-      </c>
+      <c r="AK100" s="20"/>
       <c r="AL100" s="20"/>
-      <c r="AM100" s="20" t="s">
-        <v>7</v>
-      </c>
+      <c r="AM100" s="20"/>
       <c r="AN100" s="20"/>
-      <c r="AO100" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="AO100" s="20"/>
       <c r="AP100" s="20"/>
-      <c r="AQ100" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="AQ100" s="20"/>
       <c r="AR100" s="20"/>
       <c r="AS100" s="20"/>
       <c r="AT100" s="20"/>
@@ -7270,10 +7127,10 @@
     </row>
     <row r="101" spans="1:71" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="W101" s="23" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="X101" s="23"/>
       <c r="Y101" s="23"/>
@@ -7543,56 +7400,40 @@
     </row>
     <row r="105" spans="1:71" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="R105" s="20" t="s">
         <v>71</v>
       </c>
+      <c r="R105" s="20"/>
       <c r="S105" s="20"/>
-      <c r="T105" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="T105" s="20"/>
       <c r="U105" s="20"/>
-      <c r="W105" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="W105" s="20"/>
       <c r="X105" s="20"/>
-      <c r="Y105" s="20" t="s">
-        <v>47</v>
-      </c>
+      <c r="Y105" s="20"/>
       <c r="Z105" s="20"/>
-      <c r="AB105" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="AB105" s="20"/>
       <c r="AC105" s="20"/>
-      <c r="AD105" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="AD105" s="20"/>
       <c r="AE105" s="20"/>
-      <c r="AF105" s="20" t="s">
-        <v>63</v>
-      </c>
+      <c r="AF105" s="20"/>
       <c r="AG105" s="20"/>
-      <c r="AH105" s="20" t="s">
-        <v>63</v>
-      </c>
+      <c r="AH105" s="20"/>
       <c r="AI105" s="20"/>
     </row>
     <row r="106" spans="1:71" s="12" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="R106" s="23" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="S106" s="23"/>
       <c r="T106" s="23"/>
       <c r="U106" s="23"/>
       <c r="W106" s="23" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="X106" s="23"/>
       <c r="Y106" s="23"/>
       <c r="Z106" s="23"/>
       <c r="AB106" s="23" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="AC106" s="23"/>
       <c r="AD106" s="23"/>
@@ -7677,14 +7518,14 @@
     </row>
     <row r="108" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="AG108" s="20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AH108" s="20"/>
       <c r="AI108" s="20" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AJ108" s="20"/>
       <c r="AK108" s="20" t="s">
@@ -7692,7 +7533,7 @@
       </c>
       <c r="AL108" s="20"/>
       <c r="AM108" s="20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AN108" s="20"/>
       <c r="AO108" s="20" t="s">
@@ -7700,47 +7541,47 @@
       </c>
       <c r="AP108" s="20"/>
       <c r="AQ108" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AR108" s="20"/>
       <c r="AS108" s="20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AT108" s="20"/>
       <c r="AU108" s="20" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AV108" s="20"/>
       <c r="AW108" s="20" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AX108" s="20"/>
       <c r="AY108" s="20" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="AZ108" s="20"/>
       <c r="BA108" s="20" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="BB108" s="20"/>
       <c r="BC108" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BD108" s="20"/>
       <c r="BE108" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="BF108" s="20"/>
       <c r="BG108" s="20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="BH108" s="20"/>
       <c r="BI108" s="20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="BJ108" s="20"/>
       <c r="BK108" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="BL108" s="20"/>
       <c r="BM108" s="20" t="s">
@@ -7748,7 +7589,7 @@
       </c>
       <c r="BN108" s="20"/>
       <c r="BO108" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="BP108" s="20"/>
       <c r="BQ108" s="20" t="s">
@@ -7758,10 +7599,10 @@
     </row>
     <row r="109" spans="1:71" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="AG109" s="23" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="AH109" s="23"/>
       <c r="AI109" s="23"/>
@@ -7876,7 +7717,7 @@
     </row>
     <row r="111" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="G111" s="20"/>
       <c r="H111" s="20"/>
@@ -7893,98 +7734,64 @@
       <c r="S111" s="20"/>
       <c r="T111" s="20"/>
       <c r="W111" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z111" s="20" t="s">
-        <v>61</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="Z111" s="20"/>
       <c r="AA111" s="20"/>
-      <c r="AB111" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="AB111" s="20"/>
       <c r="AC111" s="20"/>
-      <c r="AD111" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="AD111" s="20"/>
       <c r="AE111" s="20"/>
-      <c r="AF111" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="AF111" s="20"/>
       <c r="AG111" s="20"/>
-      <c r="AH111" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="AH111" s="20"/>
       <c r="AI111" s="20"/>
-      <c r="AJ111" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ111" s="20"/>
       <c r="AK111" s="20"/>
-      <c r="AL111" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="AL111" s="20"/>
       <c r="AM111" s="20"/>
-      <c r="AN111" s="20" t="s">
-        <v>61</v>
-      </c>
+      <c r="AN111" s="20"/>
       <c r="AO111" s="20"/>
-      <c r="AP111" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="AP111" s="20"/>
       <c r="AQ111" s="20"/>
       <c r="AS111" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA111" s="20" t="s">
-        <v>70</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="BA111" s="20"/>
       <c r="BB111" s="20"/>
-      <c r="BC111" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="BC111" s="20"/>
       <c r="BD111" s="20"/>
-      <c r="BF111" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="BF111" s="20"/>
       <c r="BG111" s="20"/>
-      <c r="BH111" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="BH111" s="20"/>
       <c r="BI111" s="20"/>
-      <c r="BK111" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="BK111" s="20"/>
       <c r="BL111" s="20"/>
-      <c r="BM111" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="BM111" s="20"/>
       <c r="BN111" s="20"/>
-      <c r="BO111" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="BO111" s="20"/>
       <c r="BP111" s="20"/>
-      <c r="BQ111" s="20" t="s">
-        <v>64</v>
-      </c>
+      <c r="BQ111" s="20"/>
       <c r="BR111" s="20"/>
     </row>
     <row r="112" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AS112" s="7" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="BA112" s="23" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="BB112" s="23"/>
       <c r="BC112" s="23"/>
       <c r="BD112" s="23"/>
       <c r="BF112" s="23" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="BG112" s="23"/>
       <c r="BH112" s="23"/>
       <c r="BI112" s="23"/>
       <c r="BK112" s="23" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="BL112" s="23"/>
       <c r="BM112" s="23"/>
@@ -8069,96 +7876,52 @@
     </row>
     <row r="114" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="N114" s="15"/>
-      <c r="O114" s="20" t="s">
-        <v>6</v>
-      </c>
+      <c r="O114" s="20"/>
       <c r="P114" s="20"/>
-      <c r="Q114" s="20" t="s">
-        <v>13</v>
-      </c>
+      <c r="Q114" s="20"/>
       <c r="R114" s="20"/>
-      <c r="S114" s="20" t="s">
-        <v>8</v>
-      </c>
+      <c r="S114" s="20"/>
       <c r="T114" s="20"/>
-      <c r="U114" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="U114" s="20"/>
       <c r="V114" s="20"/>
-      <c r="W114" s="20" t="s">
-        <v>102</v>
-      </c>
+      <c r="W114" s="20"/>
       <c r="X114" s="20"/>
-      <c r="Y114" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="Y114" s="20"/>
       <c r="Z114" s="20"/>
-      <c r="AA114" s="20" t="s">
-        <v>7</v>
-      </c>
+      <c r="AA114" s="20"/>
       <c r="AB114" s="20"/>
-      <c r="AC114" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="AC114" s="20"/>
       <c r="AD114" s="20"/>
-      <c r="AE114" s="20" t="s">
-        <v>6</v>
-      </c>
+      <c r="AE114" s="20"/>
       <c r="AF114" s="20"/>
-      <c r="AG114" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="AG114" s="20"/>
       <c r="AH114" s="20"/>
-      <c r="AI114" s="20" t="s">
-        <v>15</v>
-      </c>
+      <c r="AI114" s="20"/>
       <c r="AJ114" s="20"/>
-      <c r="AK114" s="20" t="s">
-        <v>21</v>
-      </c>
+      <c r="AK114" s="20"/>
       <c r="AL114" s="20"/>
-      <c r="AM114" s="20" t="s">
-        <v>6</v>
-      </c>
+      <c r="AM114" s="20"/>
       <c r="AN114" s="20"/>
-      <c r="AO114" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="AO114" s="20"/>
       <c r="AP114" s="20"/>
-      <c r="AQ114" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="AQ114" s="20"/>
       <c r="AR114" s="20"/>
-      <c r="AS114" s="20" t="s">
-        <v>6</v>
-      </c>
+      <c r="AS114" s="20"/>
       <c r="AT114" s="20"/>
-      <c r="AU114" s="20" t="s">
-        <v>24</v>
-      </c>
+      <c r="AU114" s="20"/>
       <c r="AV114" s="20"/>
-      <c r="AW114" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="AW114" s="20"/>
       <c r="AX114" s="20"/>
-      <c r="AY114" s="20" t="s">
-        <v>16</v>
-      </c>
+      <c r="AY114" s="20"/>
       <c r="AZ114" s="20"/>
-      <c r="BA114" s="20" t="s">
-        <v>15</v>
-      </c>
+      <c r="BA114" s="20"/>
       <c r="BB114" s="20"/>
-      <c r="BC114" s="20" t="s">
-        <v>7</v>
-      </c>
+      <c r="BC114" s="20"/>
       <c r="BD114" s="20"/>
-      <c r="BE114" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="BE114" s="20"/>
       <c r="BF114" s="20"/>
       <c r="BG114" s="20"/>
       <c r="BH114" s="20"/>
@@ -8481,7 +8244,7 @@
     </row>
     <row r="120" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="22" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B120" s="22"/>
       <c r="C120" s="22"/>
@@ -8775,7 +8538,7 @@
     </row>
     <row r="124" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="22" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B124" s="22"/>
       <c r="C124" s="22"/>
@@ -9142,14 +8905,14 @@
     </row>
     <row r="129" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="X129" s="20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Y129" s="20"/>
       <c r="Z129" s="20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AA129" s="20"/>
       <c r="AB129" s="20" t="s">
@@ -9157,11 +8920,11 @@
       </c>
       <c r="AC129" s="20"/>
       <c r="AD129" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AE129" s="20"/>
       <c r="AF129" s="20" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="AG129" s="20"/>
       <c r="AH129" s="20" t="s">
@@ -9241,7 +9004,7 @@
       <c r="AQ130"/>
       <c r="AR130"/>
       <c r="AS130" s="28" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="AT130" s="28"/>
       <c r="AU130" s="28"/>
@@ -9272,15 +9035,11 @@
     </row>
     <row r="131" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G131" s="20" t="s">
-        <v>61</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="G131" s="20"/>
       <c r="H131" s="20"/>
-      <c r="I131" s="20" t="s">
-        <v>62</v>
-      </c>
+      <c r="I131" s="20"/>
       <c r="J131" s="20"/>
       <c r="K131" s="20"/>
       <c r="L131" s="20"/>
@@ -9293,49 +9052,29 @@
       <c r="S131" s="20"/>
       <c r="T131" s="20"/>
       <c r="U131" s="27" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="V131" s="27"/>
       <c r="W131" s="27"/>
-      <c r="X131" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="X131" s="20"/>
       <c r="Y131" s="20"/>
-      <c r="Z131" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="Z131" s="20"/>
       <c r="AA131" s="20"/>
-      <c r="AB131" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="AB131" s="20"/>
       <c r="AC131" s="20"/>
-      <c r="AD131" s="20" t="s">
-        <v>63</v>
-      </c>
+      <c r="AD131" s="20"/>
       <c r="AE131" s="20"/>
-      <c r="AF131" s="20" t="s">
-        <v>47</v>
-      </c>
+      <c r="AF131" s="20"/>
       <c r="AG131" s="20"/>
-      <c r="AH131" s="20" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH131" s="20"/>
       <c r="AI131" s="20"/>
-      <c r="AJ131" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="AJ131" s="20"/>
       <c r="AK131" s="20"/>
-      <c r="AL131" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="AL131" s="20"/>
       <c r="AM131" s="20"/>
-      <c r="AN131" s="20" t="s">
-        <v>61</v>
-      </c>
+      <c r="AN131" s="20"/>
       <c r="AO131" s="20"/>
-      <c r="AP131" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="AP131" s="20"/>
       <c r="AQ131" s="20"/>
       <c r="AS131" s="29"/>
       <c r="AT131" s="29"/>
@@ -9344,37 +9083,21 @@
       <c r="AW131" s="29"/>
       <c r="AX131" s="29"/>
       <c r="AY131" s="29"/>
-      <c r="BA131" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="BA131" s="20"/>
       <c r="BB131" s="20"/>
-      <c r="BC131" s="20" t="s">
-        <v>64</v>
-      </c>
+      <c r="BC131" s="20"/>
       <c r="BD131" s="20"/>
-      <c r="BF131" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="BF131" s="20"/>
       <c r="BG131" s="20"/>
-      <c r="BH131" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="BH131" s="20"/>
       <c r="BI131" s="20"/>
-      <c r="BK131" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="BK131" s="20"/>
       <c r="BL131" s="20"/>
-      <c r="BM131" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="BM131" s="20"/>
       <c r="BN131" s="20"/>
-      <c r="BO131" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="BO131" s="20"/>
       <c r="BP131" s="20"/>
-      <c r="BQ131" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="BQ131" s="20"/>
       <c r="BR131" s="20"/>
     </row>
     <row r="132" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9386,19 +9109,19 @@
       <c r="AX132" s="29"/>
       <c r="AY132" s="29"/>
       <c r="BA132" s="23" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="BB132" s="23"/>
       <c r="BC132" s="23"/>
       <c r="BD132" s="23"/>
       <c r="BF132" s="23" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="BG132" s="23"/>
       <c r="BH132" s="23"/>
       <c r="BI132" s="23"/>
       <c r="BK132" s="23" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="BL132" s="23"/>
       <c r="BM132" s="23"/>
@@ -9410,116 +9133,62 @@
     </row>
     <row r="133" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="P133" s="15"/>
-      <c r="Q133" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="Q133" s="20"/>
       <c r="R133" s="20"/>
-      <c r="S133" s="20" t="s">
-        <v>13</v>
-      </c>
+      <c r="S133" s="20"/>
       <c r="T133" s="20"/>
-      <c r="U133" s="20" t="s">
-        <v>17</v>
-      </c>
+      <c r="U133" s="20"/>
       <c r="V133" s="20"/>
-      <c r="W133" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="W133" s="20"/>
       <c r="X133" s="20"/>
-      <c r="Y133" s="20" t="s">
-        <v>19</v>
-      </c>
+      <c r="Y133" s="20"/>
       <c r="Z133" s="20"/>
-      <c r="AA133" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="AA133" s="20"/>
       <c r="AB133" s="20"/>
-      <c r="AC133" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="AC133" s="20"/>
       <c r="AD133" s="20"/>
-      <c r="AE133" s="20" t="s">
-        <v>17</v>
-      </c>
+      <c r="AE133" s="20"/>
       <c r="AF133" s="20"/>
-      <c r="AG133" s="20" t="s">
-        <v>13</v>
-      </c>
+      <c r="AG133" s="20"/>
       <c r="AH133" s="20"/>
-      <c r="AI133" s="20" t="s">
-        <v>8</v>
-      </c>
+      <c r="AI133" s="20"/>
       <c r="AJ133" s="20"/>
-      <c r="AK133" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="AK133" s="20"/>
       <c r="AL133" s="20"/>
-      <c r="AM133" s="20" t="s">
-        <v>14</v>
-      </c>
+      <c r="AM133" s="20"/>
       <c r="AN133" s="20"/>
-      <c r="AO133" s="20" t="s">
-        <v>6</v>
-      </c>
+      <c r="AO133" s="20"/>
       <c r="AP133" s="20"/>
-      <c r="AQ133" s="20" t="s">
-        <v>15</v>
-      </c>
+      <c r="AQ133" s="20"/>
       <c r="AR133" s="20"/>
-      <c r="AS133" s="20" t="s">
-        <v>15</v>
-      </c>
+      <c r="AS133" s="20"/>
       <c r="AT133" s="20"/>
-      <c r="AU133" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="AU133" s="20"/>
       <c r="AV133" s="20"/>
-      <c r="AW133" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="AW133" s="20"/>
       <c r="AX133" s="20"/>
-      <c r="AY133" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="AY133" s="20"/>
       <c r="AZ133" s="20"/>
-      <c r="BA133" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="BA133" s="20"/>
       <c r="BB133" s="20"/>
-      <c r="BC133" s="20" t="s">
-        <v>6</v>
-      </c>
+      <c r="BC133" s="20"/>
       <c r="BD133" s="20"/>
-      <c r="BE133" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="BE133" s="20"/>
       <c r="BF133" s="20"/>
-      <c r="BG133" s="20" t="s">
-        <v>15</v>
-      </c>
+      <c r="BG133" s="20"/>
       <c r="BH133" s="20"/>
-      <c r="BI133" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="BI133" s="20"/>
       <c r="BJ133" s="20"/>
-      <c r="BK133" s="20" t="s">
-        <v>24</v>
-      </c>
+      <c r="BK133" s="20"/>
       <c r="BL133" s="20"/>
-      <c r="BM133" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="BM133" s="20"/>
       <c r="BN133" s="20"/>
-      <c r="BO133" s="20" t="s">
-        <v>18</v>
-      </c>
+      <c r="BO133" s="20"/>
       <c r="BP133" s="20"/>
-      <c r="BQ133" s="20" t="s">
-        <v>11</v>
-      </c>
+      <c r="BQ133" s="20"/>
       <c r="BR133" s="20"/>
     </row>
     <row r="134" spans="1:71" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9596,13 +9265,9 @@
       <c r="BS134"/>
     </row>
     <row r="135" spans="1:71" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="20" t="s">
-        <v>10</v>
-      </c>
+      <c r="A135" s="20"/>
       <c r="B135" s="20"/>
-      <c r="C135" s="20" t="s">
-        <v>6</v>
-      </c>
+      <c r="C135" s="20"/>
       <c r="D135" s="20"/>
       <c r="E135" s="20"/>
       <c r="F135" s="20"/>
@@ -9746,77 +9411,43 @@
     </row>
     <row r="137" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="N137" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="P137" s="20" t="s">
-        <v>70</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="P137" s="20"/>
       <c r="Q137" s="20"/>
-      <c r="R137" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="R137" s="20"/>
       <c r="S137" s="20"/>
-      <c r="U137" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="U137" s="20"/>
       <c r="V137" s="20"/>
-      <c r="W137" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="W137" s="20"/>
       <c r="X137" s="20"/>
-      <c r="Z137" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="Z137" s="20"/>
       <c r="AA137" s="20"/>
-      <c r="AB137" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="AB137" s="20"/>
       <c r="AC137" s="20"/>
-      <c r="AD137" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="AD137" s="20"/>
       <c r="AE137" s="20"/>
-      <c r="AF137" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="AF137" s="20"/>
       <c r="AG137" s="20"/>
-      <c r="AI137" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="AL137" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="AI137" s="7"/>
+      <c r="AL137" s="20"/>
       <c r="AM137" s="20"/>
-      <c r="AN137" s="20" t="s">
-        <v>47</v>
-      </c>
+      <c r="AN137" s="20"/>
       <c r="AO137" s="20"/>
-      <c r="AQ137" s="20" t="s">
-        <v>60</v>
-      </c>
+      <c r="AQ137" s="20"/>
       <c r="AR137" s="20"/>
-      <c r="AS137" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="AS137" s="20"/>
       <c r="AT137" s="20"/>
-      <c r="AV137" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="AV137" s="20"/>
       <c r="AW137" s="20"/>
-      <c r="AX137" s="20" t="s">
-        <v>70</v>
-      </c>
+      <c r="AX137" s="20"/>
       <c r="AY137" s="20"/>
-      <c r="AZ137" s="20" t="s">
-        <v>48</v>
-      </c>
+      <c r="AZ137" s="20"/>
       <c r="BA137" s="20"/>
-      <c r="BB137" s="20" t="s">
-        <v>71</v>
-      </c>
+      <c r="BB137" s="20"/>
       <c r="BC137" s="20"/>
     </row>
     <row r="138" spans="1:71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9836,21 +9467,21 @@
       <c r="N138"/>
       <c r="O138"/>
       <c r="P138" s="23" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="Q138" s="23"/>
       <c r="R138" s="23"/>
       <c r="S138" s="23"/>
       <c r="T138"/>
       <c r="U138" s="23" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="V138" s="23"/>
       <c r="W138" s="23"/>
       <c r="X138" s="23"/>
       <c r="Y138"/>
       <c r="Z138" s="23" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="AA138" s="23"/>
       <c r="AB138" s="23"/>
@@ -9864,21 +9495,21 @@
       <c r="AJ138"/>
       <c r="AK138"/>
       <c r="AL138" s="23" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="AM138" s="23"/>
       <c r="AN138" s="23"/>
       <c r="AO138" s="23"/>
       <c r="AP138"/>
       <c r="AQ138" s="23" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="AR138" s="23"/>
       <c r="AS138" s="23"/>
       <c r="AT138" s="23"/>
       <c r="AU138"/>
       <c r="AV138" s="23" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="AW138" s="23"/>
       <c r="AX138" s="23"/>
@@ -9906,7 +9537,7 @@
     </row>
     <row r="139" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="22" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="B139" s="22"/>
       <c r="C139" s="22"/>
@@ -10128,27 +9759,27 @@
     <row r="142" spans="1:71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="143" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="I143" s="20"/>
       <c r="J143" s="20"/>
       <c r="L143" s="7" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="R143" s="20"/>
       <c r="S143" s="20"/>
       <c r="U143" s="7" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="AA143" s="20"/>
       <c r="AB143" s="20"/>
       <c r="AD143" s="7" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="144" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="145" spans="1:71" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10588,7 +10219,7 @@
     </row>
     <row r="151" spans="1:71" s="12" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="30" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B151" s="30"/>
       <c r="C151" s="30"/>
@@ -10662,7 +10293,7 @@
     </row>
     <row r="152" spans="1:71" s="12" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="31" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B152" s="31"/>
       <c r="C152" s="31"/>
@@ -10809,7 +10440,7 @@
     </row>
     <row r="154" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="22" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B154" s="22"/>
       <c r="C154" s="22"/>
@@ -11048,7 +10679,7 @@
       <c r="Q157" s="20"/>
       <c r="R157" s="20"/>
       <c r="S157" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="T157" s="20"/>
       <c r="U157" s="20"/>
@@ -11467,7 +11098,7 @@
     </row>
     <row r="163" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="29" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B163" s="29"/>
       <c r="C163" s="29"/>
@@ -11512,24 +11143,24 @@
       <c r="AP163" s="29"/>
       <c r="AQ163" s="29"/>
       <c r="BH163" s="16" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="BJ163" s="20" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="BK163" s="20"/>
       <c r="BL163" s="32" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="BM163" s="32"/>
       <c r="BN163" s="32"/>
       <c r="BO163" s="32"/>
       <c r="BP163" s="20" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="BQ163" s="20"/>
       <c r="BR163" s="7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="164" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11699,17 +11330,17 @@
       <c r="A167" s="20"/>
       <c r="B167" s="20"/>
       <c r="D167" s="7" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="W167" s="20"/>
       <c r="X167" s="20"/>
       <c r="Z167" s="7" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="168" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z168" s="7" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
     </row>
     <row r="169" spans="1:71" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11787,7 +11418,7 @@
     </row>
     <row r="170" spans="1:71" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="29" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="B170" s="29"/>
       <c r="C170" s="29"/>
@@ -11999,19 +11630,19 @@
       <c r="AT173" s="29"/>
       <c r="AU173" s="29"/>
       <c r="AX173" s="23" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="AY173" s="23"/>
       <c r="AZ173" s="23"/>
       <c r="BA173" s="23"/>
       <c r="BC173" s="23" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="BD173" s="23"/>
       <c r="BE173" s="23"/>
       <c r="BF173" s="23"/>
       <c r="BH173" s="23" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="BI173" s="23"/>
       <c r="BJ173" s="23"/>
@@ -12096,7 +11727,7 @@
     </row>
     <row r="175" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="22" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="B175" s="22"/>
       <c r="C175" s="22"/>
@@ -12343,7 +11974,7 @@
       <c r="Y178" s="20"/>
       <c r="Z178" s="20"/>
       <c r="AA178" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AB178" s="20"/>
       <c r="AC178" s="20"/>
@@ -12363,7 +11994,7 @@
       <c r="AQ178" s="20"/>
       <c r="AR178" s="20"/>
       <c r="AS178" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AT178" s="20"/>
       <c r="AU178" s="20"/>
@@ -12466,7 +12097,7 @@
     </row>
     <row r="180" spans="1:71" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B180" s="20"/>
       <c r="C180" s="20"/>
@@ -12482,7 +12113,7 @@
       <c r="M180" s="20"/>
       <c r="N180" s="20"/>
       <c r="O180" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="P180" s="20"/>
       <c r="Q180" s="20"/>
@@ -12492,7 +12123,7 @@
       <c r="U180" s="20"/>
       <c r="V180" s="20"/>
       <c r="W180" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="X180" s="20"/>
       <c r="Y180" s="20"/>
@@ -12534,7 +12165,7 @@
       <c r="BI180" s="20"/>
       <c r="BJ180" s="20"/>
       <c r="BK180" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="BL180" s="20"/>
       <c r="BM180" s="20"/>
@@ -12546,7 +12177,7 @@
     </row>
     <row r="181" spans="1:71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="26" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B181" s="26"/>
       <c r="C181" s="26"/>
@@ -12652,7 +12283,7 @@
       <c r="AC183" s="20"/>
       <c r="AD183" s="20"/>
       <c r="AE183" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AF183" s="20"/>
       <c r="AG183" s="20"/>
@@ -12696,7 +12327,7 @@
     </row>
     <row r="184" spans="1:71" s="17" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="30" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="B184" s="30"/>
       <c r="C184" s="30"/>
@@ -12843,7 +12474,7 @@
     </row>
     <row r="186" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="22" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B186" s="22"/>
       <c r="C186" s="22"/>
@@ -13138,7 +12769,7 @@
     <row r="190" spans="1:71" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="191" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="38" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B191" s="38"/>
       <c r="C191" s="38"/>
@@ -13176,7 +12807,7 @@
       <c r="AI191" s="18"/>
       <c r="AJ191" s="18"/>
       <c r="AK191" s="38" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="AL191" s="38"/>
       <c r="AM191" s="38"/>
@@ -13215,7 +12846,7 @@
     </row>
     <row r="192" spans="1:71" s="12" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="30" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="B192" s="30"/>
       <c r="C192" s="30"/>
@@ -13290,7 +12921,7 @@
     </row>
     <row r="193" spans="1:71" s="12" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="39" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="B193" s="39"/>
       <c r="C193" s="39"/>
@@ -13438,7 +13069,7 @@
     </row>
     <row r="195" spans="1:71" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="40" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B195" s="40"/>
       <c r="C195" s="40"/>
@@ -13470,7 +13101,7 @@
       <c r="AC195" s="40"/>
       <c r="AD195" s="40"/>
       <c r="BJ195" s="41" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="BK195" s="41"/>
       <c r="BL195" s="41"/>
@@ -13557,10 +13188,10 @@
     </row>
     <row r="197" spans="1:71" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="AL197" s="35" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="AM197" s="35"/>
       <c r="AN197" s="35"/>
@@ -13670,7 +13301,7 @@
     </row>
     <row r="199" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="BJ199" s="45"/>
       <c r="BK199" s="46"/>
@@ -13758,7 +13389,7 @@
     </row>
     <row r="201" spans="1:71" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="AE201" s="33"/>
       <c r="AF201" s="33"/>
@@ -13877,7 +13508,7 @@
     </row>
     <row r="203" spans="1:71" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="G203" s="34"/>
       <c r="H203" s="34"/>
@@ -13891,7 +13522,7 @@
       <c r="P203" s="34"/>
       <c r="Q203" s="34"/>
       <c r="R203" s="35" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="S203" s="35"/>
       <c r="T203" s="35"/>
@@ -13912,7 +13543,7 @@
       <c r="AI203" s="34"/>
       <c r="AJ203" s="34"/>
       <c r="AQ203" s="16" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="AR203" s="36"/>
       <c r="AS203" s="36"/>
@@ -14018,7 +13649,7 @@
     </row>
     <row r="205" spans="1:71" s="6" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="J205" s="37"/>
       <c r="K205" s="37"/>
@@ -14084,7 +13715,7 @@
     </row>
     <row r="206" spans="1:71" s="12" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AY206" s="30" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="AZ206" s="30"/>
       <c r="BA206" s="30"/>
@@ -14109,7 +13740,7 @@
     </row>
     <row r="207" spans="1:71" s="12" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AY207" s="31" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="AZ207" s="31"/>
       <c r="BA207" s="31"/>

</xml_diff>